<commit_message>
Added Digikey part numbers and link to manufacturers webpage for 3D files
</commit_message>
<xml_diff>
--- a/docs/Alternative connectors.xlsx
+++ b/docs/Alternative connectors.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="22810"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14380" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20060" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="USB3.0" sheetId="1" r:id="rId1"/>
-    <sheet name="DIN" sheetId="2" r:id="rId2"/>
+    <sheet name="Mini-DIN" sheetId="2" r:id="rId2"/>
     <sheet name="DSUB-9" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="39">
   <si>
     <t>Port 1</t>
   </si>
@@ -74,9 +74,6 @@
     <t>GPIO8</t>
   </si>
   <si>
-    <t>DIN</t>
-  </si>
-  <si>
     <t>GPIO18</t>
   </si>
   <si>
@@ -99,6 +96,51 @@
   </si>
   <si>
     <t>Sega Master System</t>
+  </si>
+  <si>
+    <t>(GPIO17)</t>
+  </si>
+  <si>
+    <t>(GPIO18)</t>
+  </si>
+  <si>
+    <t>Digikey: 609-4663-ND</t>
+  </si>
+  <si>
+    <t>Vertical:</t>
+  </si>
+  <si>
+    <t>Horisontal:</t>
+  </si>
+  <si>
+    <t>Digikey: 609-4661-ND</t>
+  </si>
+  <si>
+    <t>Mini-DIN</t>
+  </si>
+  <si>
+    <t>Shielded:</t>
+  </si>
+  <si>
+    <t>Digikey: CP-2290-ND</t>
+  </si>
+  <si>
+    <t>Unshielded:</t>
+  </si>
+  <si>
+    <t>Digikey: CP-2490-ND</t>
+  </si>
+  <si>
+    <t>Plug (m):</t>
+  </si>
+  <si>
+    <t>Plug (f):</t>
+  </si>
+  <si>
+    <t>Digikey: CP-2090-ND</t>
+  </si>
+  <si>
+    <t>Digikey: CP-2190-ND</t>
   </si>
 </sst>
 </file>
@@ -168,7 +210,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -180,8 +222,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -199,33 +246,51 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="15"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="15" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="16">
     <cellStyle name="Följd hyperlänk" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Följd hyperlänk" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Följd hyperlänk" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Följd hyperlänk" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Följd hyperlänk" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlänk" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlänk" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlänk" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlänk" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlänk" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="15" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -290,15 +355,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -398,15 +454,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>17072</xdr:colOff>
+      <xdr:colOff>37392</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>20320</xdr:rowOff>
+      <xdr:rowOff>10160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>817880</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>172720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -429,12 +485,72 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4131872" y="254000"/>
+          <a:off x="4406192" y="243840"/>
           <a:ext cx="3269688" cy="2722880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3074" name="irc_mi" descr="//www.old-computers.com/museum/connectors/genesis_joystick.gif"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4152900" y="495300"/>
+          <a:ext cx="5080000" cy="3352800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -454,22 +570,22 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabell22" displayName="Tabell22" ref="B2:D11" totalsRowShown="0" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabell22" displayName="Tabell22" ref="B2:D11" totalsRowShown="0" headerRowDxfId="7">
   <tableColumns count="3">
-    <tableColumn id="1" name="Pin" dataDxfId="7"/>
-    <tableColumn id="2" name="Port 1" dataDxfId="6"/>
-    <tableColumn id="3" name="Port 2" dataDxfId="5"/>
+    <tableColumn id="1" name="Pin" dataDxfId="6"/>
+    <tableColumn id="2" name="Port 1" dataDxfId="5"/>
+    <tableColumn id="3" name="Port 2" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabell224" displayName="Tabell224" ref="B3:D12" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabell224" displayName="Tabell224" ref="B3:D12" totalsRowShown="0" headerRowDxfId="3">
   <tableColumns count="3">
-    <tableColumn id="1" name="Pin" dataDxfId="3"/>
-    <tableColumn id="2" name="Port 1" dataDxfId="2"/>
-    <tableColumn id="3" name="Port 2" dataDxfId="1"/>
+    <tableColumn id="1" name="Pin" dataDxfId="2"/>
+    <tableColumn id="2" name="Port 1" dataDxfId="1"/>
+    <tableColumn id="3" name="Port 2" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -730,7 +846,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -753,11 +869,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="18">
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
       <c r="E1" s="2"/>
     </row>
     <row r="2" spans="2:5">
@@ -843,8 +959,12 @@
       <c r="B9" s="4">
         <v>7</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
+      <c r="C9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="10" spans="2:5">
       <c r="B10" s="4">
@@ -865,13 +985,25 @@
         <v>14</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="2:5">
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
+      <c r="B15" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="9"/>
+    </row>
+    <row r="16" spans="2:5">
+      <c r="B16" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="19" spans="2:14">
       <c r="B19" s="3"/>
@@ -974,11 +1106,15 @@
   <mergeCells count="1">
     <mergeCell ref="B1:D1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B15" r:id="rId1"/>
+    <hyperlink ref="B16" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -990,10 +1126,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D11"/>
+  <dimension ref="B1:D18"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D11"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1003,11 +1139,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:4" ht="18">
-      <c r="B1" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
+      <c r="B1" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
     </row>
     <row r="2" spans="2:4">
       <c r="B2" s="6" t="s">
@@ -1094,7 +1230,7 @@
         <v>13</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="2:4">
@@ -1116,12 +1252,294 @@
         <v>14</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4">
+      <c r="B15" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4">
+      <c r="B16" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3">
+      <c r="B18" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:D1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B15" r:id="rId1"/>
+    <hyperlink ref="B16" r:id="rId2"/>
+    <hyperlink ref="B17" r:id="rId3"/>
+    <hyperlink ref="B18" r:id="rId4"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId5"/>
+  <tableParts count="1">
+    <tablePart r:id="rId6"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L36"/>
+  <sheetViews>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:12" ht="20">
+      <c r="A1" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+    </row>
+    <row r="2" spans="1:12" ht="18">
+      <c r="B2" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="B3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="B4" s="5">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="B5" s="4">
+        <v>2</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="B6" s="4">
+        <v>3</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="B7" s="4">
+        <v>4</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="B8" s="4">
+        <v>5</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="B9" s="4">
+        <v>6</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="B10" s="4">
+        <v>7</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="B11" s="4">
+        <v>8</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="B12" s="4">
+        <v>9</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="3"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="3"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="3"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="3"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="3"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="3"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="3"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="3"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="3"/>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="3"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="3"/>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="A1:L1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1135,248 +1553,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L36"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="1" spans="1:12" ht="20">
-      <c r="A1" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-    </row>
-    <row r="2" spans="1:12" ht="18">
-      <c r="B2" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="B3" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="B4" s="5">
-        <v>1</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="B5" s="4">
-        <v>2</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="B6" s="4">
-        <v>3</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="B7" s="4">
-        <v>4</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="B8" s="4">
-        <v>5</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
-      <c r="B9" s="4">
-        <v>6</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="B10" s="4">
-        <v>7</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
-      <c r="B11" s="4">
-        <v>8</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
-      <c r="B12" s="4">
-        <v>9</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12">
-      <c r="B16" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="3"/>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="3"/>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="3"/>
-      <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="3"/>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="3"/>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="3"/>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="3"/>
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="3"/>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="3"/>
-      <c r="B32" s="11"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="3"/>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="3"/>
-      <c r="B33" s="11"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="3"/>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="3"/>
-      <c r="B34" s="11"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="3"/>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="A1:L1"/>
-  </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <legacyDrawing r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added a skeleton for the power manager firmware
</commit_message>
<xml_diff>
--- a/docs/Alternative connectors.xlsx
+++ b/docs/Alternative connectors.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="22810"/>
   <workbookPr checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20060" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="20060"/>
   </bookViews>
   <sheets>
     <sheet name="USB3.0" sheetId="1" r:id="rId1"/>
@@ -869,7 +869,7 @@
   </sheetPr>
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
@@ -1362,7 +1362,7 @@
   </sheetPr>
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>